<commit_message>
modified:   studyNote/csapp/_labs/Lab2_bombLab/bomb/bomb.txt 	modified:   "studyNote/csapp/_labs/Lab2_bombLab/bomb/\350\215\211\347\250\277\346\234\254.xlsx"
</commit_message>
<xml_diff>
--- a/studyNote/csapp/_labs/Lab2_bombLab/bomb/草稿本.xlsx
+++ b/studyNote/csapp/_labs/Lab2_bombLab/bomb/草稿本.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monster_Liu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monster_Liu\Git\MonsterLiuNotebook\studyNote\csapp\_labs\Lab2_bombLab\bomb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6278E018-097C-4185-A3E2-55ECAD2CBD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619DB87E-72C4-45A2-8250-7E24B31E827A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="12" windowWidth="11460" windowHeight="10872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1992" yWindow="5076" windowWidth="11460" windowHeight="10872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>1 2 4 8 16 32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,6 +136,10 @@
   </si>
   <si>
     <t>rsp+48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 3 2 1 6 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -533,7 +537,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -619,7 +623,9 @@
       <c r="A6" s="2">
         <v>6</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -702,7 +708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -710,7 +716,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="3" t="s" ph="1">
         <v>13</v>
       </c>
       <c r="I14" s="1" t="s">

</xml_diff>